<commit_message>
Added NoEmail wsh.  Began adding code to EPPlusMgr to handle no-email students.
</commit_message>
<xml_diff>
--- a/iClickerQuizPtsTracker/iClickerQuizPtsTracker.xlsx
+++ b/iClickerQuizPtsTracker/iClickerQuizPtsTracker.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="7815"/>
+    <workbookView xWindow="480" yWindow="915" windowWidth="15510" windowHeight="3705" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="iClickerQuizPts" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <definedName name="rowSessionNmbr" localSheetId="0">iClickerQuizPts!$1:$1</definedName>
     <definedName name="rowTtlPts" localSheetId="0">iClickerQuizPts!$5:$5</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -346,7 +346,6 @@
     <dxf>
       <font>
         <b/>
-        <family val="2"/>
       </font>
       <alignment vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -718,7 +717,7 @@
   <sheetPr codeName="WshQuizPts"/>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="6" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
@@ -899,11 +898,12 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="WshNoEmail"/>
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:B1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,9 +920,11 @@
       </c>
     </row>
   </sheetData>
+  <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
More work on adding no-email students to ListObject.  Also adjusted code in UserControlsHandler to create BindingList of new Sessions for when there are no existing sessions.
</commit_message>
<xml_diff>
--- a/iClickerQuizPtsTracker/iClickerQuizPtsTracker.xlsx
+++ b/iClickerQuizPtsTracker/iClickerQuizPtsTracker.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bill\Documents\GitHub\iClickerQuizPtsTracker\iClickerQuizPtsTracker\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="915" windowWidth="15510" windowHeight="3705" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14700" windowHeight="7020" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="iClickerQuizPts" sheetId="1" r:id="rId1"/>
@@ -92,7 +87,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
@@ -407,7 +402,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="tblFirstQuizDts5" displayName="tblFirstQuizDts5" ref="A1:B2" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="tblNoEmail" displayName="tblNoEmail" ref="A1:B2" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A1:B2"/>
   <tableColumns count="2">
     <tableColumn id="3" name="Last Name" dataDxfId="1"/>
@@ -706,7 +701,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -903,7 +898,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Mostly finalized the code-behind for importing quiz data.
</commit_message>
<xml_diff>
--- a/iClickerQuizPtsTracker/iClickerQuizPtsTracker.xlsx
+++ b/iClickerQuizPtsTracker/iClickerQuizPtsTracker.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14700" windowHeight="7020" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14700" windowHeight="7020"/>
   </bookViews>
   <sheets>
     <sheet name="iClickerQuizPts" sheetId="1" r:id="rId1"/>
@@ -282,12 +282,33 @@
   </cellStyles>
   <dxfs count="34">
     <dxf>
+      <alignment horizontal="left" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
       <alignment horizontal="left" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -320,27 +341,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -437,43 +437,43 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="tblImpossScores" displayName="tblImpossScores" ref="A1:I2" totalsRowShown="0" headerRowDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="tblImpossScores" displayName="tblImpossScores" ref="A1:I2" totalsRowShown="0" headerRowDxfId="18">
   <autoFilter ref="A1:I2"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Student ID" dataDxfId="10"/>
-    <tableColumn id="2" name="Last Name" dataDxfId="9"/>
-    <tableColumn id="3" name="First Name" dataDxfId="8"/>
-    <tableColumn id="4" name="Course Week" dataDxfId="7"/>
-    <tableColumn id="5" name="Session" dataDxfId="6"/>
-    <tableColumn id="6" name="Quiz Date" dataDxfId="5"/>
-    <tableColumn id="7" name="Ttl Possible Points" dataDxfId="4"/>
-    <tableColumn id="8" name="Student Score" dataDxfId="3"/>
-    <tableColumn id="9" name="Score Ignored" dataDxfId="2"/>
+    <tableColumn id="1" name="Student ID" dataDxfId="17"/>
+    <tableColumn id="2" name="Last Name" dataDxfId="16"/>
+    <tableColumn id="3" name="First Name" dataDxfId="15"/>
+    <tableColumn id="4" name="Course Week" dataDxfId="14"/>
+    <tableColumn id="5" name="Session" dataDxfId="13"/>
+    <tableColumn id="6" name="Quiz Date" dataDxfId="12"/>
+    <tableColumn id="7" name="Ttl Possible Points" dataDxfId="11"/>
+    <tableColumn id="8" name="Student Score" dataDxfId="10"/>
+    <tableColumn id="9" name="Score Ignored" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="tblNoEmail" displayName="tblNoEmail" ref="A1:B2" totalsRowShown="0" headerRowDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="tblNoEmail" displayName="tblNoEmail" ref="A1:B2" totalsRowShown="0" headerRowDxfId="8">
   <autoFilter ref="A1:B2"/>
   <tableColumns count="2">
-    <tableColumn id="3" name="Last Name" dataDxfId="13"/>
-    <tableColumn id="4" name="First Name" dataDxfId="12"/>
+    <tableColumn id="3" name="Last Name" dataDxfId="7"/>
+    <tableColumn id="4" name="First Name" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="tblFirstQuizDts" displayName="tblFirstQuizDts" ref="A1:E2" totalsRowShown="0" headerRowDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="tblFirstQuizDts" displayName="tblFirstQuizDts" ref="A1:E2" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="A1:E2"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Raw iClicker Quiz File Name" dataDxfId="0"/>
-    <tableColumn id="5" name="File Date" dataDxfId="1"/>
-    <tableColumn id="2" name="Student ID" dataDxfId="17"/>
-    <tableColumn id="3" name="Last Name" dataDxfId="16"/>
-    <tableColumn id="4" name="First Name" dataDxfId="15"/>
+    <tableColumn id="1" name="Raw iClicker Quiz File Name" dataDxfId="4"/>
+    <tableColumn id="5" name="File Date" dataDxfId="3"/>
+    <tableColumn id="2" name="Student ID" dataDxfId="2"/>
+    <tableColumn id="3" name="Last Name" dataDxfId="1"/>
+    <tableColumn id="4" name="First Name" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -779,7 +779,7 @@
   <sheetPr codeName="WshQuizPts"/>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" ySplit="6" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
@@ -921,8 +921,8 @@
   <sheetPr codeName="WshImpsbScores"/>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>